<commit_message>
Retrait de struc VectorPrimitive Ajustement grille correction
</commit_message>
<xml_diff>
--- a/IFT3100H20_TP1_Grille.xlsx
+++ b/IFT3100H20_TP1_Grille.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Application\openFrameworks\apps\SlimeDungeon\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB80E96F-7ED1-4757-96A4-E61858142A2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA45C07-B785-47BC-A662-F9D81D07C900}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -473,11 +473,11 @@
     <xf numFmtId="10" fontId="2" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1674,10 +1674,10 @@
   <dimension ref="A1:IV59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1693,18 +1693,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="20.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -1790,7 +1790,7 @@
       <c r="C7" s="18">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="41" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="20"/>
@@ -1806,7 +1806,7 @@
       <c r="C8" s="18">
         <v>1.2</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="41" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="21"/>
@@ -1838,7 +1838,7 @@
       <c r="C10" s="18">
         <v>1.4</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="41" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="21"/>
@@ -1870,7 +1870,7 @@
       <c r="C12" s="18">
         <v>2.1</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="41" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="20"/>
@@ -1886,7 +1886,7 @@
       <c r="C13" s="18">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D13" s="42" t="s">
+      <c r="D13" s="41" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="21"/>
@@ -1902,7 +1902,7 @@
       <c r="C14" s="18">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="41" t="s">
         <v>15</v>
       </c>
       <c r="E14" s="20"/>
@@ -1918,7 +1918,7 @@
       <c r="C15" s="18">
         <v>2.4</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="41" t="s">
         <v>16</v>
       </c>
       <c r="E15" s="21"/>
@@ -1934,7 +1934,7 @@
       <c r="C16" s="18">
         <v>2.5</v>
       </c>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="41" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="20"/>
@@ -1950,7 +1950,7 @@
       <c r="C17" s="18">
         <v>3.1</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="41" t="s">
         <v>18</v>
       </c>
       <c r="E17" s="20"/>
@@ -1966,7 +1966,7 @@
       <c r="C18" s="18">
         <v>3.2</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="41" t="s">
         <v>19</v>
       </c>
       <c r="E18" s="21"/>
@@ -1982,7 +1982,7 @@
       <c r="C19" s="18">
         <v>3.3</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="41" t="s">
         <v>20</v>
       </c>
       <c r="E19" s="20"/>
@@ -1998,7 +1998,7 @@
       <c r="C20" s="18">
         <v>3.4</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="41" t="s">
         <v>21</v>
       </c>
       <c r="E20" s="21"/>
@@ -2062,7 +2062,7 @@
       <c r="C24" s="18">
         <v>4.3</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="41" t="s">
         <v>25</v>
       </c>
       <c r="E24" s="20"/>

</xml_diff>